<commit_message>
v 0.7 report ready
</commit_message>
<xml_diff>
--- a/excel/ts_temp.xlsx
+++ b/excel/ts_temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\teostream\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA378085-89BB-40AE-ABC5-C67FBE1DD2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1BC9C4-86FC-4540-9A88-624BC9D4E00C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2AD04834-E382-4343-AD75-E19CF9D1CEEF}"/>
   </bookViews>
@@ -60,15 +60,9 @@
     <t>Дата</t>
   </si>
   <si>
-    <t xml:space="preserve">Цель служебной поездеи </t>
-  </si>
-  <si>
     <t>Количетсво дней (включая дни отъезда/приезда, выходные и праздничные дни</t>
   </si>
   <si>
-    <t>Расходы пропроезду</t>
-  </si>
-  <si>
     <t>Расходы по найму жилого помещения</t>
   </si>
   <si>
@@ -94,13 +88,19 @@
   </si>
   <si>
     <t>Должность</t>
+  </si>
+  <si>
+    <t>Цель служебной поездки</t>
+  </si>
+  <si>
+    <t>Расходы по проезду</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +138,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,72 +155,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -225,60 +173,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -288,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -300,29 +194,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -331,22 +203,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -663,172 +532,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FF73A6-19B2-4D1A-BD3E-F54841DB571F}">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="19"/>
+        <v>16</v>
+      </c>
+      <c r="C2" s="9"/>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="79.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="D14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:7" ht="79.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="25" t="s">
+      <c r="F14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="27"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>1</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>2</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>3</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>4</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>5</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <v>6</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="12">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -836,39 +706,28 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="15"/>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -878,7 +737,7 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E15:G15"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>